<commit_message>
all components expect Rs done
</commit_message>
<xml_diff>
--- a/components.xlsx
+++ b/components.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\nixies\external\PSU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\projects\nixies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="163">
   <si>
     <t>C1</t>
   </si>
@@ -492,6 +492,27 @@
   </si>
   <si>
     <t>505-MKPX2.1/275/10P</t>
+  </si>
+  <si>
+    <t>625-ES2G-E3/5BT</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>sparkfun</t>
+  </si>
+  <si>
+    <t>871-B82477P4473M000</t>
+  </si>
+  <si>
+    <t>ALTERNATIVE TO U$2</t>
+  </si>
+  <si>
+    <t>ALTERNATIVE TO L1</t>
+  </si>
+  <si>
+    <t>used L1</t>
   </si>
 </sst>
 </file>
@@ -927,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1363,6 +1384,12 @@
       <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G22" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="6" t="s">
@@ -1482,6 +1509,9 @@
       <c r="D29" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="G29" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
@@ -1496,6 +1526,9 @@
       <c r="D30" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="G30" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
@@ -1508,19 +1541,31 @@
       <c r="D31" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="G31" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="9" t="s">
         <v>71</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1816,17 +1861,23 @@
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="9" t="s">
         <v>117</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1852,8 +1903,10 @@
     <hyperlink ref="H17" r:id="rId19" display="http://www.mouser.com/Search/ProductDetail.aspx?R=MKX21W31004B00KSSDvirtualkey50520000virtualkey505-MKPX2.1%2f275%2f10P"/>
     <hyperlink ref="H18" r:id="rId20" display="http://www.mouser.com/Search/ProductDetail.aspx?R=VJ1206V106ZXQTW1BCvirtualkey61340000virtualkey77-VJ1206V106ZXQTBC"/>
     <hyperlink ref="H19" r:id="rId21" display="http://www.mouser.com/Search/ProductDetail.aspx?R=VJ1206V106ZXQTW1BCvirtualkey61340000virtualkey77-VJ1206V106ZXQTBC"/>
+    <hyperlink ref="H22" r:id="rId22" display="http://www.mouser.com/Search/ProductDetail.aspx?R=ES2G-E3%2f5BTvirtualkey61370000virtualkey625-ES2G-E3%2f5BT"/>
+    <hyperlink ref="H32" r:id="rId23" display="http://www.mouser.com/Search/ProductDetail.aspx?R=B82477P4473M000virtualkey59250000virtualkey871-B82477P4473M000"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId22"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>